<commit_message>
Added handling of some disconnection situations
</commit_message>
<xml_diff>
--- a/Documentation/Testing V2.xlsx
+++ b/Documentation/Testing V2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zed\Desktop\SOFT564Z-CW\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AFB5A8-6774-4ABF-81EC-C1DC3AFBA801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19990F29-56A6-4218-AFC2-7E31118EE8EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>Unit</t>
   </si>
@@ -48,18 +48,6 @@
     <t>Responsible for executing code that will attempt connection to the server on click. After clicking the connect button, pattern of ip address input is verified before the connection attempt to ensure it is correct.</t>
   </si>
   <si>
-    <t>Executes code to connect to the buggy selected from the listbox.</t>
-  </si>
-  <si>
-    <t>Executes code to disconnect from the connected buggy.</t>
-  </si>
-  <si>
-    <t>Successfully connects to the buggy without any problems occurring.</t>
-  </si>
-  <si>
-    <t>Successfully disconnects from the buggy without any problems occuring.</t>
-  </si>
-  <si>
     <t>connected to buggy</t>
   </si>
   <si>
@@ -70,12 +58,6 @@
   </si>
   <si>
     <t>Connection Lost</t>
-  </si>
-  <si>
-    <t>Displays a message based on the status of the connection to the buggy. There are five types of messages that can be displayed depending on the situation. On successful connection, the controller client displays "Connected to buggy". If buggy is in use: "buggy is used by another client". On failure to connect: "Failed to connect to buggy". on loss of connection: "Connection lost". On sucessfull disconnection: "disconnected". Each condition will be presented to the controller to see how it responds.</t>
-  </si>
-  <si>
-    <t>Appropriate message should be displayed based on the presented condition.</t>
   </si>
   <si>
     <t>Used to select the interaction mode between the buggy and the controller client by the user. The controller client only enables controls associated with the chosen interaction mode.</t>
@@ -279,6 +261,87 @@
     <t xml:space="preserve">Successful connection - Units Enabled
 Failure to connect - Units disabled
 </t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>When a disconnection from the server occurs, the controller client GUI should disable all of the buggy controls to prevent the controller client from taking any action while not connected to the server. The controls that allow the usuer to connected to the server should be enabled to allow the user to try to connect back to the server.</t>
+  </si>
+  <si>
+    <t>1. Buggy controls are disabled
+2. Connect to server button is enabled
+3. Controller client disconnects from the buggy automatically.
+4. Connection status should display "Disconnected"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server Disconnection </t>
+  </si>
+  <si>
+    <t>Buggy Connection</t>
+  </si>
+  <si>
+    <t>Buggy connection button
+Buggy status textbox</t>
+  </si>
+  <si>
+    <t>Buggy interaction mode combo box</t>
+  </si>
+  <si>
+    <t>check whether the combo box will enable on scucessful connection to a buggy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successful connection - Combo box enabled
+Unscuccessful connection - Combo box disabled
+</t>
+  </si>
+  <si>
+    <t>Displays a message based on the status of the connection to the buggy. There are four types of messages that can be displayed depending on the situation. On successful connection, the controller client displays "Connected to buggy". If buggy is in use: "buggy is used by another client".  On loss of connection or failure to connect: "Disconnected".  If the user does not select a buggy to connect to: "Select a buggy to connect to".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successful Connection - Connected to buggy
+Buggy used - Buggy is used by another client
+Connection loss or inability to connect - Disconnected
+Did not select a buggy - Select a buggy to connect to
+</t>
+  </si>
+  <si>
+    <t>Buggy Disconnection</t>
+  </si>
+  <si>
+    <t>All buggy controls</t>
+  </si>
+  <si>
+    <t>Buggy Connect and Disconnect buttons</t>
+  </si>
+  <si>
+    <t>chekcs whether the buttons are appropriately disabled/enabled  on connection to a buggy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Successful connection - connect button disabled and disconnect button enabled.
+Unsuccessful connection - connect button enabled and disconnect button disabled
+</t>
+  </si>
+  <si>
+    <t>Upon disconnecting from the buggy the buggy controls apart from the buggy connection button, the status textbox and the available clients listbox should be disabled to prevent the user from generating buggy requests.</t>
+  </si>
+  <si>
+    <t>The following should be enabled only in the buggy controls:
+buggy connect button
+buggy status textbox
+available clients listbox</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Tests whether the buggy stops moving when the controller client disconnects while the buggy is set to function in 'Atuonomous Mode'</t>
+  </si>
+  <si>
+    <t>Buggy stops moving (stops autonomous mode) when controller clients disconnects from the buggy.</t>
+  </si>
+  <si>
+    <t>Picking Interaction Mode</t>
   </si>
 </sst>
 </file>
@@ -368,7 +431,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,14 +715,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="70.5703125" customWidth="1"/>
     <col min="4" max="4" width="42.85546875" customWidth="1"/>
     <col min="5" max="5" width="39.7109375" customWidth="1"/>
@@ -670,7 +733,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -692,23 +755,23 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="168" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>59</v>
+      <c r="A2" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G2" s="6">
         <v>44201</v>
@@ -716,342 +779,395 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>59</v>
+      <c r="A3" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G3" s="5">
         <v>44201</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G4" s="5">
         <v>44201</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>59</v>
+      <c r="A5" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G5" s="5">
         <v>44201</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>59</v>
+      <c r="A6" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G6" s="5">
         <v>44201</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>59</v>
+      <c r="A7" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G7" s="5">
         <v>44201</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>71</v>
+      <c r="A8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G8" s="5">
         <v>44201</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>9</v>
-      </c>
+    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>10</v>
-      </c>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="2:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3" t="s">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="D28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3" t="s">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="3:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="3:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="2:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1078,25 +1194,25 @@
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E46" s="4"/>
       <c r="H46" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E47" s="4"/>
       <c r="H47" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E48" s="4"/>
       <c r="H48" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E49" s="4"/>
       <c r="H49" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding testing writeup and more tests
</commit_message>
<xml_diff>
--- a/Documentation/Testing V2.xlsx
+++ b/Documentation/Testing V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zed\Desktop\SOFT564Z-CW\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19990F29-56A6-4218-AFC2-7E31118EE8EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446893D9-8B7D-4CA5-B5AB-FE20E3742B7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
   <si>
     <t>Unit</t>
   </si>
@@ -342,6 +342,34 @@
   </si>
   <si>
     <t>Picking Interaction Mode</t>
+  </si>
+  <si>
+    <t>Interaction Mode Combo Box
+Manual Control Focus button
+Configuration Controls
+Greenhouse data controls</t>
+  </si>
+  <si>
+    <t>Tests whether appropriate controls will enable/disable when an interaction mode is selected.</t>
+  </si>
+  <si>
+    <t>Tests whether the buggy goes into autonomous mode when the mode is selected and stops when another mode is selected</t>
+  </si>
+  <si>
+    <t>Buggy goes into autonomous mode when the mode is selected and stops working in autonomous mode when another interaction mode is selected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual Mode:
+- Control Focus Button enabled
+- Controls under greenhouse data section on the gui enabled.
+Configuration Mode:
+- Configuration controls enabled
+Autonomous Mode:
+None of the Manual, Configuration or Greenhouse data controls are enabled
+</t>
+  </si>
+  <si>
+    <t>Controlling buggy in Manual Mode</t>
   </si>
 </sst>
 </file>
@@ -715,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,39 +1028,65 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="3"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" s="3"/>
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>11</v>
       </c>
@@ -1041,7 +1095,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>13</v>
       </c>
@@ -1050,7 +1104,7 @@
       </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="3" t="s">
         <v>14</v>
       </c>
@@ -1059,7 +1113,7 @@
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C27" s="3" t="s">
         <v>15</v>
       </c>
@@ -1068,7 +1122,7 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
         <v>16</v>
       </c>
@@ -1077,7 +1131,7 @@
       </c>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="3:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>23</v>
       </c>
@@ -1086,7 +1140,7 @@
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="3:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
         <v>29</v>
       </c>
@@ -1095,7 +1149,7 @@
       </c>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="3:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
         <v>25</v>
       </c>
@@ -1104,7 +1158,7 @@
       </c>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="3:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
         <v>27</v>
       </c>

</xml_diff>